<commit_message>
update mapping scheme for Albania following local feedback (around 90% of buildings should be MUR/MCF)
</commit_message>
<xml_diff>
--- a/res_mapping_schemes/mapping_Albania_RES.xlsx
+++ b/res_mapping_schemes/mapping_Albania_RES.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10914"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAFA9BA-0C7B-9E42-AED9-18DF9A8DDA7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C68CEAC-2DA0-6C44-929C-D599F7722223}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="3340" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_urban" sheetId="5" r:id="rId1"/>
@@ -37,13 +37,6 @@
 30% CR+PC/LWAL+CDM/HBET:3-5</t>
   </si>
   <si>
-    <t>32% MUR/LWAL+CDN/H:1
-32% MCF/LWAL+CDL/H:1
-1% W/LWAL+CDL/H:1
-30% CR/LFINF+CDM/H:1
-5% CR+PC/LWAL+CDM/H:1</t>
-  </si>
-  <si>
     <t>24% MUR/LWAL+CDN/H:2
 35% MCF/LWAL+CDL/H:2
 1% W/LWAL+CDL/H:2
@@ -51,13 +44,6 @@
 10% CR+PC/LWAL+CDM/H:2</t>
   </si>
   <si>
-    <t>25% MUR/LWAL+CDN/H:1
-39% MCF/LWAL+CDL/H:1
-1% W/LWAL+CDL/H:1
-30% CR/LFINF+CDM/H:1
-5% CR+PC/LWAL+CDM/H:1</t>
-  </si>
-  <si>
     <t>23% MUR/LWAL+CDN/H:2
 30% MCF/LWAL+CDL/H:2
 1% W/LWAL+CDL/H:2
@@ -79,6 +65,16 @@
   </si>
   <si>
     <t>Number of floors</t>
+  </si>
+  <si>
+    <t>49.5% MUR/LWAL+CDN/H:1
+49.5% MCF/LWAL+CDL/H:1
+1% W/LWAL+CDL/H:1</t>
+  </si>
+  <si>
+    <t>42.5% MUR/LWAL+CDN/H:1
+56.5% MCF/LWAL+CDL/H:1
+1% W/LWAL+CDL/H:1</t>
   </si>
 </sst>
 </file>
@@ -437,7 +433,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -451,7 +447,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4">
         <v>1</v>
@@ -469,16 +465,16 @@
     <row r="2" spans="1:5" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -491,7 +487,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -505,7 +501,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="67.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="4">
         <v>1</v>
@@ -523,10 +519,10 @@
     <row r="2" spans="1:5" s="2" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>

</xml_diff>